<commit_message>
only linear interaction terms
</commit_message>
<xml_diff>
--- a/FRS_tabs.xlsx
+++ b/FRS_tabs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="460" windowWidth="26280" windowHeight="16820" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="6560" yWindow="-18820" windowWidth="26280" windowHeight="16820" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FRS - All" sheetId="2" r:id="rId1"/>
@@ -886,6 +886,11 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,11 +900,6 @@
     <xf numFmtId="2" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1221,8 +1221,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1243789440"/>
-        <c:axId val="1244210448"/>
+        <c:axId val="-840233280"/>
+        <c:axId val="-841074656"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1362,11 +1362,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1241584400"/>
-        <c:axId val="1245196704"/>
+        <c:axId val="-841067952"/>
+        <c:axId val="-841070272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1243789440"/>
+        <c:axId val="-840233280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,7 +1406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1244210448"/>
+        <c:crossAx val="-841074656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1414,7 +1414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1244210448"/>
+        <c:axId val="-841074656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="12.0"/>
@@ -1509,13 +1509,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1243789440"/>
+        <c:crossAx val="-840233280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1245196704"/>
+        <c:axId val="-841070272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.08"/>
@@ -1553,12 +1553,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1241584400"/>
+        <c:crossAx val="-841067952"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1241584400"/>
+        <c:axId val="-841067952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1245196704"/>
+        <c:crossAx val="-841070272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2573,11 +2573,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1244994784"/>
-        <c:axId val="1245128912"/>
+        <c:axId val="-840199872"/>
+        <c:axId val="-840196608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1244994784"/>
+        <c:axId val="-840199872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2620,7 +2620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1245128912"/>
+        <c:crossAx val="-840196608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2628,7 +2628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1245128912"/>
+        <c:axId val="-840196608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -2735,7 +2735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1244994784"/>
+        <c:crossAx val="-840199872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3728,11 +3728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1241595280"/>
-        <c:axId val="1241597568"/>
+        <c:axId val="-840130544"/>
+        <c:axId val="-840127280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1241595280"/>
+        <c:axId val="-840130544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,7 +3775,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1241597568"/>
+        <c:crossAx val="-840127280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3783,7 +3783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1241597568"/>
+        <c:axId val="-840127280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,7 +3834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1241595280"/>
+        <c:crossAx val="-840130544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4192,8 +4192,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1241941408"/>
-        <c:axId val="1241943728"/>
+        <c:axId val="-813661152"/>
+        <c:axId val="-813658400"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4387,11 +4387,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1242090976"/>
-        <c:axId val="1241947120"/>
+        <c:axId val="-813650880"/>
+        <c:axId val="-813654640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1241941408"/>
+        <c:axId val="-813661152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4434,7 +4434,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1241943728"/>
+        <c:crossAx val="-813658400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4442,7 +4442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1241943728"/>
+        <c:axId val="-813658400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="180.0"/>
@@ -4549,12 +4549,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1241941408"/>
+        <c:crossAx val="-813661152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1241947120"/>
+        <c:axId val="-813654640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4646,12 +4646,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242090976"/>
+        <c:crossAx val="-813650880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1242090976"/>
+        <c:axId val="-813650880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4660,7 +4660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1241947120"/>
+        <c:crossAx val="-813654640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5471,11 +5471,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1242099680"/>
-        <c:axId val="1242067632"/>
+        <c:axId val="-840982112"/>
+        <c:axId val="-840978848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1242099680"/>
+        <c:axId val="-840982112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5518,7 +5518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242067632"/>
+        <c:crossAx val="-840978848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5526,7 +5526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1242067632"/>
+        <c:axId val="-840978848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="180.0"/>
@@ -5578,7 +5578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242099680"/>
+        <c:crossAx val="-840982112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5912,11 +5912,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1242081408"/>
-        <c:axId val="1242051120"/>
+        <c:axId val="-812623856"/>
+        <c:axId val="-812621104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1242081408"/>
+        <c:axId val="-812623856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5959,7 +5959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242051120"/>
+        <c:crossAx val="-812621104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5967,7 +5967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1242051120"/>
+        <c:axId val="-812621104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6018,7 +6018,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242081408"/>
+        <c:crossAx val="-812623856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9416,7 +9416,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3814DCA5-E739-48F8-B0E6-5DAE3BD8D6DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3814DCA5-E739-48F8-B0E6-5DAE3BD8D6DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9449,7 +9449,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5CB41B8-13DC-4EAE-B2CA-47CBAE4DA728}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F5CB41B8-13DC-4EAE-B2CA-47CBAE4DA728}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9482,7 +9482,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9718F15D-DDA3-4502-9814-C910CFD7923C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9718F15D-DDA3-4502-9814-C910CFD7923C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9525,7 +9525,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEDB33E-0C98-4268-8DFA-48B4492B8054}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEDB33E-0C98-4268-8DFA-48B4492B8054}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9575,7 +9575,7 @@
         <xdr:cNvPr id="5" name="Straight Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DCBB81-D5FD-41FB-8679-A378BAA3A6A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5DCBB81-D5FD-41FB-8679-A378BAA3A6A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9625,7 +9625,7 @@
         <xdr:cNvPr id="7" name="Straight Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8871975-A065-40B2-A8DF-972697C7B8CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B8871975-A065-40B2-A8DF-972697C7B8CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9675,7 +9675,7 @@
         <xdr:cNvPr id="9" name="Straight Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40778BC-5665-464C-BFBB-9C5CBCE83F7A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A40778BC-5665-464C-BFBB-9C5CBCE83F7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9725,7 +9725,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50138399-B3EB-434F-836D-1875B4B06BE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50138399-B3EB-434F-836D-1875B4B06BE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9778,7 +9778,7 @@
         <xdr:cNvPr id="12" name="Straight Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D660D21-B51A-446B-942C-1A3FCF697F7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D660D21-B51A-446B-942C-1A3FCF697F7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9828,7 +9828,7 @@
         <xdr:cNvPr id="13" name="Straight Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{199C4030-AB22-4529-BEE1-4A656793B298}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{199C4030-AB22-4529-BEE1-4A656793B298}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9878,7 +9878,7 @@
         <xdr:cNvPr id="14" name="Freeform: Shape 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9175F49-0BEE-4CB9-BB7E-8989C18D5AF1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B9175F49-0BEE-4CB9-BB7E-8989C18D5AF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10022,7 +10022,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6799A617-2199-4FA0-9AAE-B022587C939D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6799A617-2199-4FA0-9AAE-B022587C939D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10055,7 +10055,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE41EAA9-E7EF-4331-BAC6-50A2C67981F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CE41EAA9-E7EF-4331-BAC6-50A2C67981F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10088,7 +10088,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AFBC52-30D3-4075-9EC8-31B7671415DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7AFBC52-30D3-4075-9EC8-31B7671415DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10411,10 +10411,10 @@
   <dimension ref="A1:AB105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G56" sqref="G56"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10434,26 +10434,26 @@
         <v>53</v>
       </c>
       <c r="C1" s="23"/>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="24"/>
       <c r="J1" s="24"/>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -10600,16 +10600,16 @@
       <c r="A6" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="74">
+      <c r="B6" s="71">
         <v>16.140450000000001</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="74">
+      <c r="E6" s="71">
         <v>15.07868</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="74">
+      <c r="G6" s="71">
         <v>15.15945</v>
       </c>
       <c r="H6" s="9"/>
@@ -10730,14 +10730,14 @@
       <c r="A11" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="74">
+      <c r="B11" s="71">
         <v>15.9945</v>
       </c>
-      <c r="E11" s="74">
+      <c r="E11" s="71">
         <v>15.1851</v>
       </c>
       <c r="F11" s="22"/>
-      <c r="G11" s="74">
+      <c r="G11" s="71">
         <v>15.26534</v>
       </c>
       <c r="H11" s="9"/>
@@ -10927,11 +10927,11 @@
       <c r="B18" s="52">
         <v>16.7758</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="73">
         <v>16.876090000000001</v>
       </c>
       <c r="F18" s="56"/>
-      <c r="G18" s="76">
+      <c r="G18" s="73">
         <v>17.281040000000001</v>
       </c>
       <c r="H18" s="56"/>
@@ -11102,11 +11102,11 @@
       <c r="B23" s="52">
         <v>15.64917</v>
       </c>
-      <c r="E23" s="76">
+      <c r="E23" s="73">
         <v>15.37388</v>
       </c>
       <c r="F23" s="56"/>
-      <c r="G23" s="76">
+      <c r="G23" s="73">
         <v>14.87846</v>
       </c>
       <c r="H23" s="56"/>
@@ -11261,11 +11261,11 @@
       <c r="B28" s="52">
         <v>15.62261</v>
       </c>
-      <c r="E28" s="74">
+      <c r="E28" s="71">
         <v>14.39232</v>
       </c>
       <c r="F28" s="22"/>
-      <c r="G28" s="74">
+      <c r="G28" s="71">
         <v>14.31466</v>
       </c>
       <c r="H28" s="22"/>
@@ -11407,9 +11407,9 @@
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="73"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="73"/>
+      <c r="G32" s="70"/>
       <c r="H32" s="22"/>
       <c r="K32" s="38"/>
       <c r="L32" s="38"/>
@@ -11433,11 +11433,11 @@
       <c r="B33" s="52">
         <v>15.80556</v>
       </c>
-      <c r="E33" s="74">
+      <c r="E33" s="71">
         <v>13.69</v>
       </c>
       <c r="F33" s="22"/>
-      <c r="G33" s="74">
+      <c r="G33" s="71">
         <v>13.669980000000001</v>
       </c>
       <c r="H33" s="22"/>
@@ -11615,11 +11615,11 @@
       <c r="B39" s="52">
         <v>16.628</v>
       </c>
-      <c r="E39" s="74">
+      <c r="E39" s="71">
         <v>16.800380000000001</v>
       </c>
       <c r="F39" s="22"/>
-      <c r="G39" s="74">
+      <c r="G39" s="71">
         <v>17.09845</v>
       </c>
       <c r="H39" s="22"/>
@@ -11789,11 +11789,11 @@
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
-      <c r="E44" s="75">
+      <c r="E44" s="72">
         <v>14.87846</v>
       </c>
       <c r="F44" s="57"/>
-      <c r="G44" s="75">
+      <c r="G44" s="72">
         <v>15.216570000000001</v>
       </c>
       <c r="H44" s="57"/>
@@ -11963,11 +11963,11 @@
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="74">
+      <c r="E49" s="71">
         <v>14.244</v>
       </c>
       <c r="F49" s="22"/>
-      <c r="G49" s="74">
+      <c r="G49" s="71">
         <v>14.11279</v>
       </c>
       <c r="H49" s="22"/>
@@ -12121,11 +12121,11 @@
       <c r="B54" s="52">
         <v>15.597569999999999</v>
       </c>
-      <c r="E54" s="74">
+      <c r="E54" s="71">
         <v>13.5219</v>
       </c>
       <c r="F54" s="22"/>
-      <c r="G54" s="74">
+      <c r="G54" s="71">
         <v>13.453329999999999</v>
       </c>
       <c r="H54" s="22"/>
@@ -12390,10 +12390,10 @@
       <c r="B64" s="52">
         <v>13.23739</v>
       </c>
-      <c r="E64" s="74">
+      <c r="E64" s="71">
         <v>11.243919999999999</v>
       </c>
-      <c r="G64" s="74">
+      <c r="G64" s="71">
         <v>11.59456</v>
       </c>
       <c r="H64" s="22"/>
@@ -12564,10 +12564,10 @@
       <c r="B69" s="52">
         <v>16.97439</v>
       </c>
-      <c r="E69" s="74">
+      <c r="E69" s="71">
         <v>15.730589999999999</v>
       </c>
-      <c r="G69" s="74">
+      <c r="G69" s="71">
         <v>15.552070000000001</v>
       </c>
       <c r="H69" s="22"/>
@@ -12745,10 +12745,10 @@
       <c r="B74" s="52">
         <v>19.534559999999999</v>
       </c>
-      <c r="E74" s="74">
+      <c r="E74" s="71">
         <v>18.35697</v>
       </c>
-      <c r="G74" s="74">
+      <c r="G74" s="71">
         <v>18.111979999999999</v>
       </c>
       <c r="H74" s="22"/>
@@ -13098,10 +13098,10 @@
       <c r="B85" s="52">
         <v>13.380990000000001</v>
       </c>
-      <c r="E85" s="74">
+      <c r="E85" s="71">
         <v>11.253970000000001</v>
       </c>
-      <c r="G85" s="74">
+      <c r="G85" s="71">
         <v>11.59909</v>
       </c>
       <c r="H85" s="22"/>
@@ -13271,10 +13271,10 @@
       <c r="B90" s="52">
         <v>16.91761</v>
       </c>
-      <c r="E90" s="74">
+      <c r="E90" s="71">
         <v>15.73494</v>
       </c>
-      <c r="G90" s="74">
+      <c r="G90" s="71">
         <v>15.5692</v>
       </c>
       <c r="H90" s="22"/>
@@ -13434,11 +13434,11 @@
       </c>
       <c r="C95" s="22"/>
       <c r="D95" s="22"/>
-      <c r="E95" s="74">
+      <c r="E95" s="71">
         <v>18.378430000000002</v>
       </c>
       <c r="F95" s="22"/>
-      <c r="G95" s="74">
+      <c r="G95" s="71">
         <v>18.110900000000001</v>
       </c>
       <c r="H95" s="22"/>
@@ -13546,7 +13546,7 @@
       <c r="A98" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="B98" s="77" t="s">
+      <c r="B98" s="74" t="s">
         <v>111</v>
       </c>
       <c r="C98" s="22"/>
@@ -13597,16 +13597,16 @@
       <c r="A100" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B100" s="77" t="s">
+      <c r="B100" s="74" t="s">
         <v>111</v>
       </c>
       <c r="C100" s="22"/>
       <c r="D100" s="22"/>
-      <c r="E100" s="77" t="s">
+      <c r="E100" s="74" t="s">
         <v>111</v>
       </c>
       <c r="F100" s="57"/>
-      <c r="G100" s="77" t="s">
+      <c r="G100" s="74" t="s">
         <v>111</v>
       </c>
       <c r="H100" s="57"/>
@@ -13713,18 +13713,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
@@ -14488,23 +14488,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="F1" s="70" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="F1" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
       <c r="R1" s="9"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -15556,83 +15556,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="R1" s="72" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="R1" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AF1" s="72" t="s">
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AF1" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
-      <c r="AK1" s="72"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="72"/>
-      <c r="AN1" s="72"/>
-      <c r="AO1" s="72"/>
-      <c r="AP1" s="72"/>
-      <c r="AQ1" s="72"/>
-      <c r="AR1" s="72"/>
-      <c r="AT1" s="72" t="s">
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="77"/>
+      <c r="AT1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="AU1" s="72"/>
-      <c r="AV1" s="72"/>
-      <c r="AW1" s="72"/>
-      <c r="AX1" s="72"/>
-      <c r="AY1" s="72"/>
-      <c r="AZ1" s="72"/>
-      <c r="BA1" s="72"/>
-      <c r="BB1" s="72"/>
-      <c r="BC1" s="72"/>
-      <c r="BD1" s="72"/>
-      <c r="BE1" s="72"/>
-      <c r="BF1" s="72"/>
-      <c r="BH1" s="72" t="s">
+      <c r="AU1" s="77"/>
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="77"/>
+      <c r="AX1" s="77"/>
+      <c r="AY1" s="77"/>
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="77"/>
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="77"/>
+      <c r="BH1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="BI1" s="72"/>
-      <c r="BJ1" s="72"/>
-      <c r="BK1" s="72"/>
-      <c r="BL1" s="72"/>
-      <c r="BM1" s="72"/>
-      <c r="BN1" s="72"/>
-      <c r="BO1" s="72"/>
-      <c r="BP1" s="72"/>
-      <c r="BQ1" s="72"/>
-      <c r="BR1" s="72"/>
-      <c r="BS1" s="72"/>
-      <c r="BT1" s="72"/>
+      <c r="BI1" s="77"/>
+      <c r="BJ1" s="77"/>
+      <c r="BK1" s="77"/>
+      <c r="BL1" s="77"/>
+      <c r="BM1" s="77"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="77"/>
+      <c r="BP1" s="77"/>
+      <c r="BQ1" s="77"/>
+      <c r="BR1" s="77"/>
+      <c r="BS1" s="77"/>
+      <c r="BT1" s="77"/>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>

</xml_diff>